<commit_message>
Proche de la fin
je corrige calcul avec group plus simple puisque on a pas a verifier que group sur meme slot E
finalement la limite pompe peu facilement se mettre dans CtoP
ajout de filtre pour colonne 
ajout de widget pour plus de figure
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DD2C23-8833-49A7-9CAD-1D18E44AD8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97865B-AD54-4669-8635-61D9F7FF344D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +547,7 @@
     <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -581,8 +581,9 @@
       <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -614,7 +615,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -634,7 +635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -666,7 +667,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -692,7 +693,7 @@
         <v>7.6400000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -712,7 +713,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -738,7 +739,7 @@
         <v>2.3499999999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -758,7 +759,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -775,7 +776,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -798,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -815,7 +816,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -832,7 +833,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -849,7 +850,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
@@ -869,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
bew func for generate indiv by name and notebook test
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97865B-AD54-4669-8635-61D9F7FF344D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EFF1B7-91D2-42BC-96C7-71C5BADAAC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="137">
   <si>
     <t>Composants</t>
   </si>
@@ -201,13 +203,259 @@
   </si>
   <si>
     <t>ramp</t>
+  </si>
+  <si>
+    <t>Strat</t>
+  </si>
+  <si>
+    <t>Full_s</t>
+  </si>
+  <si>
+    <t>full g</t>
+  </si>
+  <si>
+    <t>gr E1</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Group Capteur</t>
+  </si>
+  <si>
+    <t>No Group Capteur s</t>
+  </si>
+  <si>
+    <t>Pression debit C0</t>
+  </si>
+  <si>
+    <t>[2.23, 36.31]</t>
+  </si>
+  <si>
+    <t>[1.95, 33.94]</t>
+  </si>
+  <si>
+    <t>[5.2, 55.49]</t>
+  </si>
+  <si>
+    <t>[4.45, 51.34]</t>
+  </si>
+  <si>
+    <t>[1.30, 27.78]</t>
+  </si>
+  <si>
+    <t>[2.84, 41.04]</t>
+  </si>
+  <si>
+    <t>[2.94, 9.04]</t>
+  </si>
+  <si>
+    <t>[6.72, 13.67]</t>
+  </si>
+  <si>
+    <t>Pression debit C1</t>
+  </si>
+  <si>
+    <t>[4.48, 11.15]</t>
+  </si>
+  <si>
+    <t>[4.14, 10.73]</t>
+  </si>
+  <si>
+    <t>[11.01, 17.49]</t>
+  </si>
+  <si>
+    <t>[10.02, 16.68]</t>
+  </si>
+  <si>
+    <t>Pression debit C2</t>
+  </si>
+  <si>
+    <t>[4.51, 11.19]</t>
+  </si>
+  <si>
+    <t>[2.97, 9.08]</t>
+  </si>
+  <si>
+    <t>[11.09, 17.55]</t>
+  </si>
+  <si>
+    <t>[6.8, 13.74]</t>
+  </si>
+  <si>
+    <t>[1.34, 28.19]</t>
+  </si>
+  <si>
+    <t>[2.93, 41.63]</t>
+  </si>
+  <si>
+    <t>[1.99, 34.31]</t>
+  </si>
+  <si>
+    <t>[4.54, 51.87]</t>
+  </si>
+  <si>
+    <t>Pression debit C3</t>
+  </si>
+  <si>
+    <t>[4.51, 11.20]</t>
+  </si>
+  <si>
+    <t>[4.18, 10.77]</t>
+  </si>
+  <si>
+    <t>[11.10, 17.56]</t>
+  </si>
+  <si>
+    <t>[10.11, 16.75]</t>
+  </si>
+  <si>
+    <t>[2.30, 36.91]</t>
+  </si>
+  <si>
+    <t>[5.36, 56.36]</t>
+  </si>
+  <si>
+    <t>Debit total</t>
+  </si>
+  <si>
+    <t>69.85</t>
+  </si>
+  <si>
+    <t>64.52</t>
+  </si>
+  <si>
+    <t>65.37</t>
+  </si>
+  <si>
+    <t>108.09</t>
+  </si>
+  <si>
+    <t>98.51</t>
+  </si>
+  <si>
+    <t>100.13</t>
+  </si>
+  <si>
+    <t>78.32</t>
+  </si>
+  <si>
+    <t>117.72</t>
+  </si>
+  <si>
+    <t>91.41</t>
+  </si>
+  <si>
+    <t>139.39</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>pompe</t>
+  </si>
+  <si>
+    <t>0 1 2 3</t>
+  </si>
+  <si>
+    <t>0 2</t>
+  </si>
+  <si>
+    <t>1 3</t>
+  </si>
+  <si>
+    <t>gr E2</t>
+  </si>
+  <si>
+    <t>[1.46, 29.43]</t>
+  </si>
+  <si>
+    <t>[5.20, 55.49]</t>
+  </si>
+  <si>
+    <t>[3.23, 43.73]</t>
+  </si>
+  <si>
+    <t>[4.48, 11.16]</t>
+  </si>
+  <si>
+    <t>[2.22, 7.85]</t>
+  </si>
+  <si>
+    <t>[11.02, 17.50]</t>
+  </si>
+  <si>
+    <t>[4.9, 11.67]0</t>
+  </si>
+  <si>
+    <t>[9.99, 16.66]</t>
+  </si>
+  <si>
+    <t>[2.23, 7.88]</t>
+  </si>
+  <si>
+    <t>[2.973, 9.08]</t>
+  </si>
+  <si>
+    <t>[4.93, 11.70]</t>
+  </si>
+  <si>
+    <t>[4.46, 11.13]</t>
+  </si>
+  <si>
+    <t>[2.21, 7.83]</t>
+  </si>
+  <si>
+    <t>[10.96, 17.45]</t>
+  </si>
+  <si>
+    <t>[4.87, 11.63]</t>
+  </si>
+  <si>
+    <t>[9.93, 16.61]</t>
+  </si>
+  <si>
+    <t>69.79</t>
+  </si>
+  <si>
+    <t>52.99</t>
+  </si>
+  <si>
+    <t>65.31</t>
+  </si>
+  <si>
+    <t>107.99</t>
+  </si>
+  <si>
+    <t>78.73</t>
+  </si>
+  <si>
+    <t>100.03</t>
+  </si>
+  <si>
+    <t>106.31</t>
+  </si>
+  <si>
+    <t>78.26</t>
+  </si>
+  <si>
+    <t>117.62</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,16 +469,76 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF82E600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7981D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7E1CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -238,17 +546,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,4 +1256,962 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54961E9C-4C47-48F5-A8A6-030F2C9B75E5}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="11" width="17.140625" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="13">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <v>3</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9EAFC-E6C4-49D8-8E7F-104277C8EC1C}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="13">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>3</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
reprise split & PF test
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EFF1B7-91D2-42BC-96C7-71C5BADAAC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A869A5-A848-4DA5-9A78-CEDC95DF6509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="confs" sheetId="1" r:id="rId1"/>
+    <sheet name="map" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="map (2)" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="166">
   <si>
     <t>Composants</t>
   </si>
@@ -449,13 +453,100 @@
   </si>
   <si>
     <t>117.62</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>g3p</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>R, F, F, F</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>0,1,2,3</t>
+  </si>
+  <si>
+    <t>(0,2),(1,3)</t>
+  </si>
+  <si>
+    <t>0, (1,2) ,3</t>
+  </si>
+  <si>
+    <t>0, (1,2) , 3</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>(0,1,2),3</t>
+  </si>
+  <si>
+    <t>pression</t>
+  </si>
+  <si>
+    <t>2.2, 4.4, 4.5, 4.4</t>
+  </si>
+  <si>
+    <t>2.2, 4.1, 4.1, 4.4</t>
+  </si>
+  <si>
+    <t>debit</t>
+  </si>
+  <si>
+    <t>36.3, 11.1, 11.1, 11.1</t>
+  </si>
+  <si>
+    <t>36,3, 10.7, 10.7, 11.1</t>
+  </si>
+  <si>
+    <t>debit total</t>
+  </si>
+  <si>
+    <t>69.7</t>
+  </si>
+  <si>
+    <t>65.3</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>E4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,8 +566,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -537,8 +634,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAD1DC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D2E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -561,11 +676,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -610,6 +740,27 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1259,6 +1410,299 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F29B31-6C0D-40B3-B31D-F123035F6D9E}">
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="5.28515625" style="13" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="13">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="13">
+        <v>1</v>
+      </c>
+      <c r="F1" s="13">
+        <v>1</v>
+      </c>
+      <c r="G1" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:G10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54961E9C-4C47-48F5-A8A6-030F2C9B75E5}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -1760,12 +2204,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9EAFC-E6C4-49D8-8E7F-104277C8EC1C}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,4 +2658,907 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F764EC02-E99F-482E-990B-B17D1B85CFBB}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="13">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13">
+        <v>3</v>
+      </c>
+      <c r="D1" s="13">
+        <v>4</v>
+      </c>
+      <c r="E1" s="13">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13">
+        <v>6</v>
+      </c>
+      <c r="G1" s="13">
+        <v>7</v>
+      </c>
+      <c r="H1" s="13">
+        <v>8</v>
+      </c>
+      <c r="I1" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480DF4AE-546A-448B-B7CA-289C7BCE992B}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.5703125" style="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="16">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16">
+        <v>2</v>
+      </c>
+      <c r="E1" s="16">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="17">
+        <v>1</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17">
+        <v>1</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C3ECA9-050A-4ABB-904A-776388DE759D}">
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="5.28515625" style="13" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="13">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="13">
+        <v>1</v>
+      </c>
+      <c r="F1" s="13">
+        <v>1</v>
+      </c>
+      <c r="G1" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:G10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>